<commit_message>
Solo 1 tabla con datos de pacientes y permisos actualizados
</commit_message>
<xml_diff>
--- a/Jorge Diego Manrique/Definición usuarios.xlsx
+++ b/Jorge Diego Manrique/Definición usuarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\GitHub\Datos-Epilepsia-2021\Jorge Diego Manrique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5746880-4334-4A0D-8FA0-E282DBC9772F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A41E5-A792-492C-95CE-35788D115142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8175" yWindow="2385" windowWidth="17640" windowHeight="11055" xr2:uid="{09960BBC-791D-4C4A-86A7-0BCEF8ED93A5}"/>
+    <workbookView xWindow="7245" yWindow="8205" windowWidth="17640" windowHeight="9450" xr2:uid="{09960BBC-791D-4C4A-86A7-0BCEF8ED93A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Administrador</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Todas las tablas de la bd.</t>
   </si>
   <si>
-    <t>A toda las tablas menos a pacientes_datos_personales.</t>
-  </si>
-  <si>
-    <t>*Dependiendo si los datos se separan en 2 tablas o se emplea seguridad por columna.</t>
-  </si>
-  <si>
     <t>Privilegios</t>
   </si>
   <si>
@@ -69,8 +63,17 @@
     <t>Solo puede consultar (Select)</t>
   </si>
   <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Todos las db y sus tablas.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Todos (create, drop, delete, insert, select, update) </t>
+      <t>Solo puede actualizar, insertar y consultar datos en las tablas ya creadas.</t>
     </r>
     <r>
       <rPr>
@@ -81,8 +84,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>o mejor solo insert, update y select?</t>
+      <t xml:space="preserve"> (</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Insert, update y select)</t>
+    </r>
+  </si>
+  <si>
+    <t>Todas la tablas pero no a las columnas con datos confidenciales del paciente.</t>
+  </si>
+  <si>
+    <t>La tabla "pacientes" contiene columnas confidenciales.</t>
   </si>
 </sst>
 </file>
@@ -445,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E865866-EF4E-4B78-9F9B-509577440023}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,52 +480,63 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>